<commit_message>
arreglo excel, y mediciones en metros superiores a 500m incluye poligono de referencia
</commit_message>
<xml_diff>
--- a/puntos_actualizados.xlsx
+++ b/puntos_actualizados.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>archivo_json</t>
+          <t>nombre_poligono</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -582,18 +582,22 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>black</t>
+          <t>red</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>No_poligono</t>
+          <t>Fuera</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>443.605998775727</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>29_2.json</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -708,7 +712,11 @@
       <c r="H7" t="n">
         <v>5539.313632921418</v>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -741,7 +749,11 @@
       <c r="H8" t="n">
         <v>6414.816381557062</v>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -774,7 +786,11 @@
       <c r="H9" t="n">
         <v>5029.671456606073</v>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -807,7 +823,11 @@
       <c r="H10" t="n">
         <v>1336.783636890868</v>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -840,7 +860,11 @@
       <c r="H11" t="n">
         <v>1439.082676239756</v>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -873,7 +897,11 @@
       <c r="H12" t="n">
         <v>1575.434084835697</v>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -947,7 +975,11 @@
       <c r="H14" t="n">
         <v>4930.99673875148</v>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1021,7 +1053,11 @@
       <c r="H16" t="n">
         <v>4773.045531251983</v>
       </c>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1054,7 +1090,11 @@
       <c r="H17" t="n">
         <v>6430.092839645848</v>
       </c>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1087,7 +1127,11 @@
       <c r="H18" t="n">
         <v>32307.87495150493</v>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1120,7 +1164,11 @@
       <c r="H19" t="n">
         <v>32330.91647159238</v>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1153,7 +1201,11 @@
       <c r="H20" t="n">
         <v>32370.02624607358</v>
       </c>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1186,7 +1238,11 @@
       <c r="H21" t="n">
         <v>32355.39886003724</v>
       </c>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1219,7 +1275,11 @@
       <c r="H22" t="n">
         <v>32355.39886003724</v>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1252,7 +1312,11 @@
       <c r="H23" t="n">
         <v>31981.20562567628</v>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1285,7 +1349,11 @@
       <c r="H24" t="n">
         <v>31970.37525957975</v>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1318,7 +1386,11 @@
       <c r="H25" t="n">
         <v>18701.83844412884</v>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1351,7 +1423,11 @@
       <c r="H26" t="n">
         <v>22106.18855402583</v>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1384,7 +1460,11 @@
       <c r="H27" t="n">
         <v>22350.58086311822</v>
       </c>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1417,7 +1497,11 @@
       <c r="H28" t="n">
         <v>22359.61462312678</v>
       </c>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1450,7 +1534,11 @@
       <c r="H29" t="n">
         <v>576.8273959403749</v>
       </c>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1483,7 +1571,11 @@
       <c r="H30" t="n">
         <v>619.2014479550551</v>
       </c>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1516,7 +1608,11 @@
       <c r="H31" t="n">
         <v>576.762799338669</v>
       </c>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2406_0.json</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1549,7 +1645,11 @@
       <c r="H32" t="n">
         <v>744.8634575932665</v>
       </c>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2406_0.json</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1623,7 +1723,11 @@
       <c r="H34" t="n">
         <v>7698.237720147124</v>
       </c>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1857,7 +1961,11 @@
       <c r="H40" t="n">
         <v>6355.618272092917</v>
       </c>
-      <c r="I40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1890,7 +1998,11 @@
       <c r="H41" t="n">
         <v>1528.302444436419</v>
       </c>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1923,7 +2035,11 @@
       <c r="H42" t="n">
         <v>1384.642554261193</v>
       </c>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1956,7 +2072,11 @@
       <c r="H43" t="n">
         <v>1293.93107943285</v>
       </c>
-      <c r="I43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2026,7 +2146,11 @@
       <c r="H45" t="n">
         <v>7885.780354635473</v>
       </c>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2920,7 +3044,11 @@
       <c r="H67" t="n">
         <v>257816.4977305467</v>
       </c>
-      <c r="I67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2953,7 +3081,11 @@
       <c r="H68" t="n">
         <v>257718.2975359401</v>
       </c>
-      <c r="I68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2986,7 +3118,11 @@
       <c r="H69" t="n">
         <v>257887.605948064</v>
       </c>
-      <c r="I69" t="inlineStr"/>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3019,7 +3155,11 @@
       <c r="H70" t="n">
         <v>309008.703004736</v>
       </c>
-      <c r="I70" t="inlineStr"/>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3052,7 +3192,11 @@
       <c r="H71" t="n">
         <v>309417.5186686103</v>
       </c>
-      <c r="I71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3085,7 +3229,11 @@
       <c r="H72" t="n">
         <v>308493.5722840882</v>
       </c>
-      <c r="I72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3282,7 +3430,11 @@
       <c r="H77" t="n">
         <v>266641.1603563711</v>
       </c>
-      <c r="I77" t="inlineStr"/>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3315,7 +3467,11 @@
       <c r="H78" t="n">
         <v>265823.3091396675</v>
       </c>
-      <c r="I78" t="inlineStr"/>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3419,18 +3575,22 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>black</t>
+          <t>red</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>No_poligono</t>
+          <t>Fuera</t>
         </is>
       </c>
       <c r="H81" t="n">
         <v>443.605998775727</v>
       </c>
-      <c r="I81" t="inlineStr"/>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>29_2.json</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3545,7 +3705,11 @@
       <c r="H84" t="n">
         <v>5539.313632921418</v>
       </c>
-      <c r="I84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3578,7 +3742,11 @@
       <c r="H85" t="n">
         <v>6414.816381557062</v>
       </c>
-      <c r="I85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3611,7 +3779,11 @@
       <c r="H86" t="n">
         <v>5029.671456606073</v>
       </c>
-      <c r="I86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3644,7 +3816,11 @@
       <c r="H87" t="n">
         <v>1336.783636890868</v>
       </c>
-      <c r="I87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3677,7 +3853,11 @@
       <c r="H88" t="n">
         <v>1439.082676239756</v>
       </c>
-      <c r="I88" t="inlineStr"/>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3710,7 +3890,11 @@
       <c r="H89" t="n">
         <v>1575.434084835697</v>
       </c>
-      <c r="I89" t="inlineStr"/>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3825,7 +4009,11 @@
       <c r="H92" t="n">
         <v>4930.99673875148</v>
       </c>
-      <c r="I92" t="inlineStr"/>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3899,7 +4087,11 @@
       <c r="H94" t="n">
         <v>4773.045531251983</v>
       </c>
-      <c r="I94" t="inlineStr"/>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3932,7 +4124,11 @@
       <c r="H95" t="n">
         <v>6430.092839645848</v>
       </c>
-      <c r="I95" t="inlineStr"/>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3965,7 +4161,11 @@
       <c r="H96" t="n">
         <v>32307.87495150493</v>
       </c>
-      <c r="I96" t="inlineStr"/>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3998,7 +4198,11 @@
       <c r="H97" t="n">
         <v>32334.15519636469</v>
       </c>
-      <c r="I97" t="inlineStr"/>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4031,7 +4235,11 @@
       <c r="H98" t="n">
         <v>32370.02624607358</v>
       </c>
-      <c r="I98" t="inlineStr"/>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4064,7 +4272,11 @@
       <c r="H99" t="n">
         <v>32355.39886003724</v>
       </c>
-      <c r="I99" t="inlineStr"/>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4097,7 +4309,11 @@
       <c r="H100" t="n">
         <v>31981.20562567628</v>
       </c>
-      <c r="I100" t="inlineStr"/>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4130,7 +4346,11 @@
       <c r="H101" t="n">
         <v>31970.37525957975</v>
       </c>
-      <c r="I101" t="inlineStr"/>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4163,7 +4383,11 @@
       <c r="H102" t="n">
         <v>18665.6226620853</v>
       </c>
-      <c r="I102" t="inlineStr"/>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4196,7 +4420,11 @@
       <c r="H103" t="n">
         <v>19004.83406435666</v>
       </c>
-      <c r="I103" t="inlineStr"/>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4229,7 +4457,11 @@
       <c r="H104" t="n">
         <v>22106.18855402583</v>
       </c>
-      <c r="I104" t="inlineStr"/>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4262,7 +4494,11 @@
       <c r="H105" t="n">
         <v>22350.58086311822</v>
       </c>
-      <c r="I105" t="inlineStr"/>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4295,7 +4531,11 @@
       <c r="H106" t="n">
         <v>22359.61462312678</v>
       </c>
-      <c r="I106" t="inlineStr"/>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>31000_13.json</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4328,7 +4568,11 @@
       <c r="H107" t="n">
         <v>32330.91647159238</v>
       </c>
-      <c r="I107" t="inlineStr"/>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>1257_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4361,7 +4605,11 @@
       <c r="H108" t="n">
         <v>576.762799338669</v>
       </c>
-      <c r="I108" t="inlineStr"/>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2406_0.json</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4394,7 +4642,11 @@
       <c r="H109" t="n">
         <v>744.8634575932665</v>
       </c>
-      <c r="I109" t="inlineStr"/>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2406_0.json</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4468,7 +4720,11 @@
       <c r="H111" t="n">
         <v>7698.237720147124</v>
       </c>
-      <c r="I111" t="inlineStr"/>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4702,7 +4958,11 @@
       <c r="H117" t="n">
         <v>1956.789297620546</v>
       </c>
-      <c r="I117" t="inlineStr"/>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2406_0.json</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4735,7 +4995,11 @@
       <c r="H118" t="n">
         <v>6355.618272092917</v>
       </c>
-      <c r="I118" t="inlineStr"/>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>354_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4768,7 +5032,11 @@
       <c r="H119" t="n">
         <v>1528.302444436419</v>
       </c>
-      <c r="I119" t="inlineStr"/>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4801,7 +5069,11 @@
       <c r="H120" t="n">
         <v>1384.642554261193</v>
       </c>
-      <c r="I120" t="inlineStr"/>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4834,7 +5106,11 @@
       <c r="H121" t="n">
         <v>1293.93107943285</v>
       </c>
-      <c r="I121" t="inlineStr"/>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2700_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5806,7 +6082,11 @@
       <c r="H145" t="n">
         <v>257816.4977305467</v>
       </c>
-      <c r="I145" t="inlineStr"/>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5839,7 +6119,11 @@
       <c r="H146" t="n">
         <v>257718.2975359401</v>
       </c>
-      <c r="I146" t="inlineStr"/>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5872,7 +6156,11 @@
       <c r="H147" t="n">
         <v>257887.605948064</v>
       </c>
-      <c r="I147" t="inlineStr"/>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5905,7 +6193,11 @@
       <c r="H148" t="n">
         <v>309008.703004736</v>
       </c>
-      <c r="I148" t="inlineStr"/>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5938,7 +6230,11 @@
       <c r="H149" t="n">
         <v>309417.5186686103</v>
       </c>
-      <c r="I149" t="inlineStr"/>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5971,7 +6267,11 @@
       <c r="H150" t="n">
         <v>308493.5722840882</v>
       </c>
-      <c r="I150" t="inlineStr"/>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6168,7 +6468,11 @@
       <c r="H155" t="n">
         <v>266641.1603563711</v>
       </c>
-      <c r="I155" t="inlineStr"/>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6201,7 +6505,11 @@
       <c r="H156" t="n">
         <v>265823.3091396675</v>
       </c>
-      <c r="I156" t="inlineStr"/>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6234,7 +6542,11 @@
       <c r="H157" t="n">
         <v>265804.9344128223</v>
       </c>
-      <c r="I157" t="inlineStr"/>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>46_52.json</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6267,7 +6579,11 @@
       <c r="H158" t="n">
         <v>537.5405677916909</v>
       </c>
-      <c r="I158" t="inlineStr"/>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>1361_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6378,7 +6694,11 @@
       <c r="H161" t="n">
         <v>797.1602168018983</v>
       </c>
-      <c r="I161" t="inlineStr"/>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>1361_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6534,7 +6854,11 @@
       <c r="H165" t="n">
         <v>882.9832669643304</v>
       </c>
-      <c r="I165" t="inlineStr"/>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6567,7 +6891,11 @@
       <c r="H166" t="n">
         <v>934.4359100018157</v>
       </c>
-      <c r="I166" t="inlineStr"/>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6600,7 +6928,11 @@
       <c r="H167" t="n">
         <v>537.5405677916909</v>
       </c>
-      <c r="I167" t="inlineStr"/>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>1361_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6711,7 +7043,11 @@
       <c r="H170" t="n">
         <v>797.1602168018983</v>
       </c>
-      <c r="I170" t="inlineStr"/>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>1361_1.json</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6744,7 +7080,11 @@
       <c r="H171" t="n">
         <v>722.212417653418</v>
       </c>
-      <c r="I171" t="inlineStr"/>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6777,7 +7117,11 @@
       <c r="H172" t="n">
         <v>719.1331563547607</v>
       </c>
-      <c r="I172" t="inlineStr"/>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6966,7 +7310,11 @@
       <c r="H177" t="n">
         <v>882.9832669643304</v>
       </c>
-      <c r="I177" t="inlineStr"/>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6999,7 +7347,11 @@
       <c r="H178" t="n">
         <v>934.4359100018157</v>
       </c>
-      <c r="I178" t="inlineStr"/>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>847_3.json</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">

</xml_diff>